<commit_message>
Fixed bug in significance analysis
There was a bug that was causing a lot of the number of significant cells to default to 5. That was fixed and data was re-output.
</commit_message>
<xml_diff>
--- a/Paper Rebuttal/Adjustments_12_2019/Data/results_significance_N_first_10.xlsx
+++ b/Paper Rebuttal/Adjustments_12_2019/Data/results_significance_N_first_10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lccam\Documents\CU Boulder\Donaldson Lab\Imaging-Paper\Paper Rebuttal\Adjustments_12_2019\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7A9997E-7AB7-4006-8419-0EE5FCD23A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF132561-3BA6-43DD-B87A-CEB40BCB9941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{830EAB70-514D-46A8-A83B-21DB2AADF4C0}"/>
   </bookViews>
@@ -534,16 +534,16 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.45454545454545453</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="M2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>0.45454545454545453</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="O2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -557,22 +557,22 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>0.29411764705882354</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.29411764705882354</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="G3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0.29411764705882354</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -639,34 +639,34 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0.10869565217391304</v>
+        <v>2.1739130434782608E-2</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>0.10869565217391304</v>
+        <v>6.5217391304347824E-2</v>
       </c>
       <c r="I5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J5">
-        <v>0.10869565217391304</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="K5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>0.10869565217391304</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="M5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N5">
-        <v>0.10869565217391304</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -680,10 +680,10 @@
         <v>38</v>
       </c>
       <c r="D6">
-        <v>0.13157894736842105</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6">
         <v>0.21052631578947367</v>
@@ -698,16 +698,16 @@
         <v>9</v>
       </c>
       <c r="J6">
-        <v>0.13157894736842105</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="K6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L6">
-        <v>0.13157894736842105</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N6">
         <v>0.13157894736842105</v>
@@ -727,40 +727,40 @@
         <v>30</v>
       </c>
       <c r="D7">
-        <v>0.16666666666666666</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>0.16666666666666666</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>0.16666666666666666</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7">
-        <v>0.16666666666666666</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0.16666666666666666</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="M7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N7">
-        <v>0.16666666666666666</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="O7">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -774,10 +774,10 @@
         <v>56</v>
       </c>
       <c r="D8">
-        <v>8.9285714285714288E-2</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8">
         <v>8.9285714285714288E-2</v>
@@ -897,22 +897,22 @@
         <v>9</v>
       </c>
       <c r="J11">
-        <v>0.15151515151515152</v>
+        <v>3.0303030303030304E-2</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>0.15151515151515152</v>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="M11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N11">
-        <v>0.15151515151515152</v>
+        <v>0.12121212121212122</v>
       </c>
       <c r="O11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -926,16 +926,16 @@
         <v>38</v>
       </c>
       <c r="D12">
-        <v>0.13157894736842105</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F12">
-        <v>0.13157894736842105</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12">
         <v>0.18421052631578946</v>
@@ -944,22 +944,22 @@
         <v>7</v>
       </c>
       <c r="J12">
-        <v>0.13157894736842105</v>
+        <v>2.6315789473684209E-2</v>
       </c>
       <c r="K12">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.13157894736842105</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="M12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N12">
-        <v>0.13157894736842105</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -973,34 +973,34 @@
         <v>28</v>
       </c>
       <c r="D13">
-        <v>0.17857142857142858</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.17857142857142858</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>0.17857142857142858</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J13">
-        <v>0.17857142857142858</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="K13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L13">
-        <v>0.17857142857142858</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N13">
         <v>0.21428571428571427</v>
@@ -1020,40 +1020,40 @@
         <v>23</v>
       </c>
       <c r="D14">
-        <v>0.21739130434782608</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>0.21739130434782608</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>0.21739130434782608</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>0.21739130434782608</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="K14">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L14">
-        <v>0.21739130434782608</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="M14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N14">
-        <v>0.21739130434782608</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="O14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1067,34 +1067,34 @@
         <v>24</v>
       </c>
       <c r="D15">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H15">
-        <v>0.20833333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="I15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15">
-        <v>0.20833333333333334</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="K15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
       <c r="M15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N15">
         <v>0.20833333333333334</v>
@@ -1114,22 +1114,22 @@
         <v>28</v>
       </c>
       <c r="D16">
-        <v>0.17857142857142858</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F16">
-        <v>0.17857142857142858</v>
+        <v>0.10714285714285714</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>0.17857142857142858</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="I16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1144,10 +1144,10 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0.17857142857142858</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="O16">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1161,16 +1161,16 @@
         <v>17</v>
       </c>
       <c r="D17">
-        <v>0.29411764705882354</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>0.29411764705882354</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>0.29411764705882354</v>
@@ -1179,22 +1179,22 @@
         <v>5</v>
       </c>
       <c r="J17">
-        <v>0.29411764705882354</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="K17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L17">
-        <v>0.29411764705882354</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="M17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N17">
-        <v>0.29411764705882354</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="O17">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1226,22 +1226,22 @@
         <v>7</v>
       </c>
       <c r="J18">
-        <v>0.27777777777777779</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="K18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0.27777777777777779</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>0.27777777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="O18">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1273,22 +1273,22 @@
         <v>22</v>
       </c>
       <c r="J19">
-        <v>0.12195121951219512</v>
+        <v>2.4390243902439025E-2</v>
       </c>
       <c r="K19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L19">
-        <v>0.12195121951219512</v>
+        <v>2.4390243902439025E-2</v>
       </c>
       <c r="M19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N19">
-        <v>0.12195121951219512</v>
+        <v>4.878048780487805E-2</v>
       </c>
       <c r="O19">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1326,10 +1326,10 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0.10204081632653061</v>
+        <v>8.1632653061224483E-2</v>
       </c>
       <c r="M20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N20">
         <v>0.14285714285714285</v>
@@ -1349,10 +1349,10 @@
         <v>40</v>
       </c>
       <c r="D21">
-        <v>0.125</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <v>0.15</v>
@@ -1367,22 +1367,22 @@
         <v>14</v>
       </c>
       <c r="J21">
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0.125</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="M21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N21">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="O21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1396,10 +1396,10 @@
         <v>42</v>
       </c>
       <c r="D22">
-        <v>0.11904761904761904</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F22">
         <v>0.16666666666666666</v>
@@ -1414,16 +1414,16 @@
         <v>8</v>
       </c>
       <c r="J22">
-        <v>0.11904761904761904</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="K22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L22">
-        <v>0.11904761904761904</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="M22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N22">
         <v>0.23809523809523808</v>
@@ -1496,16 +1496,16 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="M24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N24">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="O24">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -1624,10 +1624,10 @@
         <v>23</v>
       </c>
       <c r="D28">
-        <v>0.21739130434782608</v>
+        <v>8.6956521739130432E-2</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F28">
         <v>0.21739130434782608</v>
@@ -1654,10 +1654,10 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.21739130434782608</v>
+        <v>4.3478260869565216E-2</v>
       </c>
       <c r="O28">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1689,22 +1689,22 @@
         <v>9</v>
       </c>
       <c r="J29">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="K29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L29">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="M29">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N29">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O29">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1736,22 +1736,22 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0.27777777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="K30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L30">
-        <v>0.27777777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="M30">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N30">
-        <v>0.27777777777777779</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="O30">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1783,22 +1783,22 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>0.38461538461538464</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="K31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L31">
-        <v>0.38461538461538464</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="M31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N31">
-        <v>0.38461538461538464</v>
+        <v>0.23076923076923078</v>
       </c>
       <c r="O31">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -1812,16 +1812,16 @@
         <v>57</v>
       </c>
       <c r="D32">
-        <v>8.771929824561403E-2</v>
+        <v>1.7543859649122806E-2</v>
       </c>
       <c r="E32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>8.771929824561403E-2</v>
+        <v>3.5087719298245612E-2</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>0.10526315789473684</v>
@@ -1830,10 +1830,10 @@
         <v>6</v>
       </c>
       <c r="J32">
-        <v>8.771929824561403E-2</v>
+        <v>1.7543859649122806E-2</v>
       </c>
       <c r="K32">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L32">
         <v>8.771929824561403E-2</v>
@@ -1894,16 +1894,16 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0.15151515151515152</v>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="G34">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H34">
-        <v>0.15151515151515152</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -1918,10 +1918,10 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0.15151515151515152</v>
+        <v>6.0606060606060608E-2</v>
       </c>
       <c r="O34">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -1970,28 +1970,28 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H36">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="I36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J36">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="K36">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L36">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="M36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N36">
         <v>0.3</v>
@@ -2029,22 +2029,22 @@
         <v>0</v>
       </c>
       <c r="J37">
-        <v>0.3125</v>
+        <v>6.25E-2</v>
       </c>
       <c r="K37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L37">
-        <v>0.3125</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N37">
-        <v>0.3125</v>
+        <v>0.125</v>
       </c>
       <c r="O37">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -2082,16 +2082,16 @@
         <v>0</v>
       </c>
       <c r="L38">
-        <v>0.38461538461538464</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="M38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N38">
-        <v>0.38461538461538464</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="O38">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -2111,16 +2111,16 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0.38461538461538464</v>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <v>0.38461538461538464</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="I39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2135,10 +2135,10 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.38461538461538464</v>
+        <v>0.15384615384615385</v>
       </c>
       <c r="O39">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -2164,28 +2164,28 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J40">
-        <v>0.17241379310344829</v>
+        <v>3.4482758620689655E-2</v>
       </c>
       <c r="K40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L40">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="M40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N40">
-        <v>0.17241379310344829</v>
+        <v>0.13793103448275862</v>
       </c>
       <c r="O40">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -2199,16 +2199,16 @@
         <v>39</v>
       </c>
       <c r="D41">
-        <v>0.12820512820512819</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>0.12820512820512819</v>
+        <v>0.10256410256410256</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H41">
         <v>0.15384615384615385</v>
@@ -2217,16 +2217,16 @@
         <v>6</v>
       </c>
       <c r="J41">
-        <v>0.12820512820512819</v>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="K41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L41">
-        <v>0.12820512820512819</v>
+        <v>0.10256410256410256</v>
       </c>
       <c r="M41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N41">
         <v>0.15384615384615385</v>
@@ -2246,16 +2246,16 @@
         <v>68</v>
       </c>
       <c r="D42">
-        <v>7.3529411764705885E-2</v>
+        <v>2.9411764705882353E-2</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F42">
-        <v>7.3529411764705885E-2</v>
+        <v>4.4117647058823532E-2</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H42">
         <v>8.8235294117647065E-2</v>
@@ -2264,10 +2264,10 @@
         <v>6</v>
       </c>
       <c r="J42">
-        <v>7.3529411764705885E-2</v>
+        <v>4.4117647058823532E-2</v>
       </c>
       <c r="K42">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L42">
         <v>7.3529411764705885E-2</v>
@@ -2311,10 +2311,10 @@
         <v>8</v>
       </c>
       <c r="J43">
-        <v>5.4945054945054944E-2</v>
+        <v>3.2967032967032968E-2</v>
       </c>
       <c r="K43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L43">
         <v>5.4945054945054944E-2</v>
@@ -2340,22 +2340,22 @@
         <v>19</v>
       </c>
       <c r="D44">
-        <v>0.26315789473684209</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F44">
-        <v>0.26315789473684209</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="G44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H44">
-        <v>0.26315789473684209</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="I44">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -2364,16 +2364,16 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <v>0.26315789473684209</v>
+        <v>5.2631578947368418E-2</v>
       </c>
       <c r="M44">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N44">
-        <v>0.26315789473684209</v>
+        <v>0.15789473684210525</v>
       </c>
       <c r="O44">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -2405,22 +2405,22 @@
         <v>12</v>
       </c>
       <c r="J45">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="K45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L45">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="M45">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N45">
-        <v>0.17241379310344829</v>
+        <v>0.10344827586206896</v>
       </c>
       <c r="O45">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -2434,34 +2434,34 @@
         <v>22</v>
       </c>
       <c r="D46">
-        <v>0.22727272727272727</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>0.22727272727272727</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="G46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>0.22727272727272727</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="I46">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J46">
-        <v>0.22727272727272727</v>
+        <v>4.5454545454545456E-2</v>
       </c>
       <c r="K46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L46">
-        <v>0.22727272727272727</v>
+        <v>0.13636363636363635</v>
       </c>
       <c r="M46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N46">
         <v>0.22727272727272727</v>
@@ -2481,34 +2481,34 @@
         <v>36</v>
       </c>
       <c r="D47">
-        <v>0.1388888888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="E47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>0.1388888888888889</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H47">
-        <v>0.1388888888888889</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="I47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J47">
-        <v>0.1388888888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="K47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L47">
-        <v>0.1388888888888889</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="M47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N47">
         <v>0.1388888888888889</v>
@@ -2528,28 +2528,28 @@
         <v>47</v>
       </c>
       <c r="D48">
-        <v>0.10638297872340426</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="E48">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F48">
-        <v>0.10638297872340426</v>
+        <v>6.3829787234042548E-2</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H48">
-        <v>0.10638297872340426</v>
+        <v>8.5106382978723402E-2</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J48">
-        <v>0.10638297872340426</v>
+        <v>4.2553191489361701E-2</v>
       </c>
       <c r="K48">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L48">
         <v>0.1276595744680851</v>
@@ -2575,10 +2575,10 @@
         <v>53</v>
       </c>
       <c r="D49">
-        <v>9.4339622641509441E-2</v>
+        <v>5.6603773584905662E-2</v>
       </c>
       <c r="E49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F49">
         <v>0.11320754716981132</v>
@@ -2599,16 +2599,16 @@
         <v>0</v>
       </c>
       <c r="L49">
-        <v>9.4339622641509441E-2</v>
+        <v>1.8867924528301886E-2</v>
       </c>
       <c r="M49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N49">
-        <v>9.4339622641509441E-2</v>
+        <v>7.5471698113207544E-2</v>
       </c>
       <c r="O49">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -2628,34 +2628,34 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0.10638297872340426</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H50">
-        <v>0.10638297872340426</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="I50">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J50">
-        <v>0.10638297872340426</v>
+        <v>4.2553191489361701E-2</v>
       </c>
       <c r="K50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L50">
-        <v>0.10638297872340426</v>
+        <v>4.2553191489361701E-2</v>
       </c>
       <c r="M50">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N50">
-        <v>0.10638297872340426</v>
+        <v>6.3829787234042548E-2</v>
       </c>
       <c r="O50">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -2681,22 +2681,22 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0.11904761904761904</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="I51">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J51">
-        <v>0.11904761904761904</v>
+        <v>7.1428571428571425E-2</v>
       </c>
       <c r="K51">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L51">
-        <v>0.11904761904761904</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="M51">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N51">
         <v>0.14285714285714285</v>
@@ -2716,40 +2716,40 @@
         <v>40</v>
       </c>
       <c r="D52">
-        <v>0.125</v>
+        <v>0.05</v>
       </c>
       <c r="E52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F52">
-        <v>0.125</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H52">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="I52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J52">
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="K52">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L52">
-        <v>0.125</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="M52">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N52">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="O52">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -2763,16 +2763,16 @@
         <v>36</v>
       </c>
       <c r="D53">
-        <v>0.1388888888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="E53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F53">
-        <v>0.1388888888888889</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H53">
         <v>0.16666666666666666</v>
@@ -2793,10 +2793,10 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <v>0.1388888888888889</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="O53">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -2810,40 +2810,40 @@
         <v>38</v>
       </c>
       <c r="D54">
-        <v>0.13157894736842105</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F54">
-        <v>0.13157894736842105</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="G54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H54">
-        <v>0.13157894736842105</v>
+        <v>0.10526315789473684</v>
       </c>
       <c r="I54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J54">
-        <v>0.13157894736842105</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="K54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L54">
-        <v>0.13157894736842105</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="M54">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N54">
-        <v>0.13157894736842105</v>
+        <v>7.8947368421052627E-2</v>
       </c>
       <c r="O54">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -2875,22 +2875,22 @@
         <v>8</v>
       </c>
       <c r="J55">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="K55">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L55">
-        <v>0.17241379310344829</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="M55">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N55">
-        <v>0.17241379310344829</v>
+        <v>0.10344827586206896</v>
       </c>
       <c r="O55">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>